<commit_message>
27-09-18 (Aug->Sept fix + garagabezoek)
</commit_message>
<xml_diff>
--- a/Ritgegevens.xlsx
+++ b/Ritgegevens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TGR\Desktop\Administratie\Ritgegevens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DE09DA-5A93-499A-92B4-B2AFBF3028F4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFF1A3C-4753-4697-AC11-F76A1796EA09}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{E1CDE313-428E-477A-B89C-B5B20550DB53}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Zuiderhoofdstraat 32, Krommenie</t>
+  </si>
+  <si>
+    <t>Veluwezoom 4, 1327AG, Almere</t>
+  </si>
+  <si>
+    <t>Garagebezoek, inclusief proefrit monteur</t>
   </si>
 </sst>
 </file>
@@ -536,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6C79BF-5DF7-4F63-ABB9-74D4FAF6D5B0}">
   <dimension ref="A1:K547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,7 +1482,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
-        <v>43327</v>
+        <v>43358</v>
       </c>
       <c r="B29" s="6">
         <v>1371</v>
@@ -1541,7 +1547,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>43329</v>
+        <v>43360</v>
       </c>
       <c r="B31" s="6">
         <v>1396</v>
@@ -1606,7 +1612,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
-        <v>43330</v>
+        <v>43361</v>
       </c>
       <c r="B33" s="6">
         <v>1531</v>
@@ -1672,7 +1678,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
-        <v>43331</v>
+        <v>43362</v>
       </c>
       <c r="B35" s="6">
         <v>1666</v>
@@ -1738,7 +1744,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
-        <v>43332</v>
+        <v>43363</v>
       </c>
       <c r="B37" s="6">
         <v>1801</v>
@@ -1804,7 +1810,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
-        <v>43336</v>
+        <v>43367</v>
       </c>
       <c r="B39" s="6">
         <v>1936</v>
@@ -1843,25 +1849,25 @@
       </c>
       <c r="C40" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2052</v>
       </c>
       <c r="D40" s="8" t="str">
         <f t="shared" si="4"/>
         <v>Duwboot 20, Houten</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="6">
         <f t="shared" si="5"/>
-        <v>-2004</v>
+        <v>48</v>
       </c>
       <c r="J40" s="6">
         <f t="shared" si="2"/>
-        <v>-2004</v>
+        <v>48</v>
       </c>
       <c r="K40" s="6">
         <f t="shared" si="3"/>
@@ -1870,26 +1876,30 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
+      <c r="B41" s="6">
+        <v>2052</v>
+      </c>
       <c r="C41" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2095</v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>De Boeg 26, Zaandam</v>
-      </c>
-      <c r="E41" s="8"/>
+        <v>Veluwezoom 4, 1327AG, Almere</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="G41" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I41" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J41" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K41" s="6">
         <f t="shared" si="3"/>
@@ -1897,55 +1907,67 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="5">
+        <v>43368</v>
+      </c>
+      <c r="B42" s="6">
+        <v>2095</v>
+      </c>
       <c r="C42" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D42" s="8">
+        <v>2162</v>
+      </c>
+      <c r="D42" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E42" s="8"/>
+        <v>De Boeg 26, Zaandam</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="G42" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I42" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J42" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K42" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
+      <c r="B43" s="6">
+        <v>2162</v>
+      </c>
       <c r="C43" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="8">
+        <v>2165</v>
+      </c>
+      <c r="D43" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="8"/>
+        <v>Duwboot 20, Houten</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="G43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I43" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J43" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K43" s="6">
         <f t="shared" si="3"/>
@@ -1954,26 +1976,30 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
+      <c r="B44" s="6">
+        <v>2165</v>
+      </c>
       <c r="C44" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D44" s="8">
+        <v>2231</v>
+      </c>
+      <c r="D44" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="8"/>
+        <v>Waterveste 4, Houten</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="G44" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I44" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="J44" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="K44" s="6">
         <f t="shared" si="3"/>
@@ -1981,27 +2007,33 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="5">
+        <v>43370</v>
+      </c>
+      <c r="B45" s="6">
+        <v>2231</v>
+      </c>
       <c r="C45" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D45" s="8">
+        <v>2298</v>
+      </c>
+      <c r="D45" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="8"/>
+        <v>De Boeg 26, Zaandam</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="G45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I45" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J45" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K45" s="6">
         <f t="shared" si="3"/>
@@ -2010,26 +2042,30 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
+      <c r="B46" s="6">
+        <v>2298</v>
+      </c>
       <c r="C46" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="8"/>
+        <v>Duwboot 20, Houten</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="G46" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I46" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-2298</v>
       </c>
       <c r="J46" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-2298</v>
       </c>
       <c r="K46" s="6">
         <f t="shared" si="3"/>
@@ -2043,9 +2079,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>De Boeg 26, Zaandam</v>
       </c>
       <c r="E47" s="8"/>
       <c r="G47" s="4" t="s">

</xml_diff>